<commit_message>
fix bug and add function splitby
</commit_message>
<xml_diff>
--- a/IN/Book1.xlsx
+++ b/IN/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>MAKH</t>
   </si>
@@ -90,19 +90,31 @@
   </si>
   <si>
     <t>DFG</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>VKORG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,8 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,15 +422,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C50"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +441,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3560</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -431,7 +452,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3560</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -439,7 +463,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3550</v>
+      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -447,7 +474,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3550</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -455,7 +485,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3560</v>
+      </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -463,7 +496,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3550</v>
+      </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -471,7 +507,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3560</v>
+      </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -479,7 +518,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3550</v>
+      </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -487,7 +529,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3560</v>
+      </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -495,7 +540,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3550</v>
+      </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -503,7 +551,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3560</v>
+      </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -511,7 +562,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3560</v>
+      </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -519,7 +573,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3560</v>
+      </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -527,7 +584,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3550</v>
+      </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -535,7 +595,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3550</v>
+      </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
@@ -543,7 +606,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3560</v>
+      </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -551,7 +617,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3550</v>
+      </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
@@ -559,7 +628,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3560</v>
+      </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -567,7 +639,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3550</v>
+      </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -575,7 +650,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3560</v>
+      </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -583,7 +661,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3550</v>
+      </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -591,7 +672,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3550</v>
+      </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -599,7 +683,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3550</v>
+      </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -607,7 +694,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3560</v>
+      </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -615,7 +705,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3550</v>
+      </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -623,7 +716,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3560</v>
+      </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -631,7 +727,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3550</v>
+      </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
@@ -639,7 +738,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3550</v>
+      </c>
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -647,7 +749,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3560</v>
+      </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
@@ -655,7 +760,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3550</v>
+      </c>
       <c r="B31" t="s">
         <v>16</v>
       </c>
@@ -663,12 +771,21 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3550</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
       <c r="C32">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3550</v>
+      </c>
       <c r="B33" t="s">
         <v>17</v>
       </c>
@@ -676,7 +793,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3550</v>
+      </c>
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -684,7 +804,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3560</v>
+      </c>
       <c r="B35" t="s">
         <v>18</v>
       </c>
@@ -692,7 +815,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3550</v>
+      </c>
       <c r="B36" t="s">
         <v>17</v>
       </c>
@@ -700,7 +826,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3560</v>
+      </c>
       <c r="B37" t="s">
         <v>14</v>
       </c>
@@ -708,7 +837,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3550</v>
+      </c>
       <c r="B38" t="s">
         <v>19</v>
       </c>
@@ -716,7 +848,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3560</v>
+      </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
@@ -724,7 +859,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3560</v>
+      </c>
       <c r="B40" t="s">
         <v>20</v>
       </c>
@@ -732,7 +870,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3550</v>
+      </c>
       <c r="B41" t="s">
         <v>20</v>
       </c>
@@ -740,7 +881,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3550</v>
+      </c>
       <c r="B42" t="s">
         <v>20</v>
       </c>
@@ -748,7 +892,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3560</v>
+      </c>
       <c r="B43" t="s">
         <v>20</v>
       </c>
@@ -756,7 +903,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3560</v>
+      </c>
       <c r="B44" t="s">
         <v>20</v>
       </c>
@@ -764,7 +914,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3550</v>
+      </c>
       <c r="B45" t="s">
         <v>20</v>
       </c>
@@ -772,7 +925,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3560</v>
+      </c>
       <c r="B46" t="s">
         <v>20</v>
       </c>
@@ -780,7 +936,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3560</v>
+      </c>
       <c r="B47" t="s">
         <v>20</v>
       </c>
@@ -788,7 +947,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3560</v>
+      </c>
       <c r="B48" t="s">
         <v>21</v>
       </c>
@@ -796,7 +958,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3560</v>
+      </c>
       <c r="B49" t="s">
         <v>20</v>
       </c>
@@ -804,7 +969,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3560</v>
+      </c>
       <c r="B50" t="s">
         <v>20</v>
       </c>

</xml_diff>